<commit_message>
Added new data to matlab file
</commit_message>
<xml_diff>
--- a/startingpointanalysisnoredpoints_04120.xlsx
+++ b/startingpointanalysisnoredpoints_04120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713F1303-E840-488C-A5CD-A3CF0B04482E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A180F-B9A4-4A9E-A80A-38F667A2A1EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B2391AF-3C98-487A-A35E-AC8619BBF83F}"/>
   </bookViews>
@@ -41,12 +41,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,9 +67,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,15 +388,15 @@
   <dimension ref="A1:V132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -448,9 +455,11 @@
         <f>SQRT(P1^2+Q1^2+R1^2)</f>
         <v>0.23576161738571866</v>
       </c>
-      <c r="V1" s="1"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V1" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2.0450312385911232E-2</v>
       </c>
@@ -509,9 +518,11 @@
         <f t="shared" ref="T2:T65" si="0">SQRT(P2^2+Q2^2+R2^2)</f>
         <v>0.1992197658356884</v>
       </c>
-      <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -570,9 +581,11 @@
         <f t="shared" si="0"/>
         <v>0.22519938449748692</v>
       </c>
-      <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V3" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -631,9 +644,11 @@
         <f t="shared" si="0"/>
         <v>0.30857770223530995</v>
       </c>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.9831237033261315E-2</v>
       </c>
@@ -692,9 +707,11 @@
         <f t="shared" si="0"/>
         <v>0.24684821224360323</v>
       </c>
-      <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V5" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.9740589692919586E-2</v>
       </c>
@@ -753,9 +770,11 @@
         <f t="shared" si="0"/>
         <v>0.25234270910007206</v>
       </c>
-      <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V6" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -814,9 +833,11 @@
         <f t="shared" si="0"/>
         <v>1.3711248730011278</v>
       </c>
-      <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V7" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -875,9 +896,11 @@
         <f t="shared" si="0"/>
         <v>1.3759482195072894</v>
       </c>
-      <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V8" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -936,9 +959,11 @@
         <f t="shared" si="0"/>
         <v>1.3747700717895857</v>
       </c>
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V9" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -997,9 +1022,11 @@
         <f t="shared" si="0"/>
         <v>1.3720242596480909</v>
       </c>
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V10" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -1058,9 +1085,11 @@
         <f t="shared" si="0"/>
         <v>1.3648343324924233</v>
       </c>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V11" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.0274801300881475E-2</v>
       </c>
@@ -1119,9 +1148,11 @@
         <f t="shared" si="0"/>
         <v>0.28536335563239623</v>
       </c>
-      <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.1119872308029211E-2</v>
       </c>
@@ -1180,9 +1211,11 @@
         <f t="shared" si="0"/>
         <v>0.27653304805554874</v>
       </c>
-      <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.9910210046424383E-2</v>
       </c>
@@ -1241,9 +1274,11 @@
         <f t="shared" si="0"/>
         <v>0.26697795581775102</v>
       </c>
-      <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.9620662521692256E-2</v>
       </c>
@@ -1302,9 +1337,11 @@
         <f t="shared" si="0"/>
         <v>0.25689831194217183</v>
       </c>
-      <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.9764000132085034E-2</v>
       </c>
@@ -1363,9 +1400,11 @@
         <f t="shared" si="0"/>
         <v>0.24627356997130229</v>
       </c>
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V16" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.9778014887334602E-2</v>
       </c>
@@ -1424,9 +1463,11 @@
         <f t="shared" si="0"/>
         <v>0.2359338351674849</v>
       </c>
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V17" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2.0031222373319477E-2</v>
       </c>
@@ -1485,9 +1526,11 @@
         <f t="shared" si="0"/>
         <v>0.23626966325917489</v>
       </c>
-      <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.9970275304346936E-2</v>
       </c>
@@ -1546,9 +1589,11 @@
         <f t="shared" si="0"/>
         <v>0.38766555965981697</v>
       </c>
-      <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V19" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.9717191812744631E-2</v>
       </c>
@@ -1607,9 +1652,11 @@
         <f t="shared" si="0"/>
         <v>0.50779738075644765</v>
       </c>
-      <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V20" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.9975017608702555E-2</v>
       </c>
@@ -1668,9 +1715,11 @@
         <f t="shared" si="0"/>
         <v>0.64267044310010668</v>
       </c>
-      <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V21" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.0025153872303574E-2</v>
       </c>
@@ -1729,9 +1778,11 @@
         <f t="shared" si="0"/>
         <v>0.76629016277011019</v>
       </c>
-      <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V22" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.960784313729759E-2</v>
       </c>
@@ -1790,9 +1841,11 @@
         <f t="shared" si="0"/>
         <v>0.73188781575891648</v>
       </c>
-      <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V23" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.9607843137290287E-2</v>
       </c>
@@ -1851,9 +1904,11 @@
         <f t="shared" si="0"/>
         <v>0.72457965847632111</v>
       </c>
-      <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V24" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.960784313762608E-2</v>
       </c>
@@ -1912,9 +1967,11 @@
         <f t="shared" si="0"/>
         <v>0.71674691497675636</v>
       </c>
-      <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V25" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2.0463363330335108E-2</v>
       </c>
@@ -1973,9 +2030,11 @@
         <f t="shared" si="0"/>
         <v>0.7105831315879455</v>
       </c>
-      <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V26" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1.9770622156745334E-2</v>
       </c>
@@ -2034,9 +2093,11 @@
         <f t="shared" si="0"/>
         <v>0.70008591319710556</v>
       </c>
-      <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V27" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -2095,9 +2156,11 @@
         <f t="shared" si="0"/>
         <v>0.73204930090700981</v>
       </c>
-      <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V28" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1.960784315901512E-2</v>
       </c>
@@ -2156,9 +2219,11 @@
         <f t="shared" si="0"/>
         <v>0.71655838841047192</v>
       </c>
-      <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V29" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1.962108131661346E-2</v>
       </c>
@@ -2217,9 +2282,11 @@
         <f t="shared" si="0"/>
         <v>0.72707787724745232</v>
       </c>
-      <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V30" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -2278,9 +2345,11 @@
         <f t="shared" si="0"/>
         <v>1.2955427244581841</v>
       </c>
-      <c r="V31" s="1"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V31" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -2339,9 +2408,11 @@
         <f t="shared" si="0"/>
         <v>0.93560762871730452</v>
       </c>
-      <c r="V32" s="1"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V32" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -2400,9 +2471,11 @@
         <f t="shared" si="0"/>
         <v>0.76354013658370312</v>
       </c>
-      <c r="V33" s="1"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V33" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2.0017697070074295E-2</v>
       </c>
@@ -2461,9 +2534,11 @@
         <f t="shared" si="0"/>
         <v>0.2793882481869317</v>
       </c>
-      <c r="V34" s="1"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V34" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2.0008754759221273E-2</v>
       </c>
@@ -2522,9 +2597,11 @@
         <f t="shared" si="0"/>
         <v>0.23532878180639241</v>
       </c>
-      <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V35" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2.0048138991549846E-2</v>
       </c>
@@ -2583,9 +2660,11 @@
         <f t="shared" si="0"/>
         <v>0.2669179108104866</v>
       </c>
-      <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V36" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.9998353406495858E-2</v>
       </c>
@@ -2644,9 +2723,11 @@
         <f t="shared" si="0"/>
         <v>0.27107300220372271</v>
       </c>
-      <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V37" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1.9931135700434449E-2</v>
       </c>
@@ -2705,9 +2786,11 @@
         <f t="shared" si="0"/>
         <v>0.25348219814501483</v>
       </c>
-      <c r="V38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V38" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1.9708024936159696E-2</v>
       </c>
@@ -2766,9 +2849,11 @@
         <f t="shared" si="0"/>
         <v>0.23988562604985394</v>
       </c>
-      <c r="V39" s="1"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V39" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1.9649699966683469E-2</v>
       </c>
@@ -2827,9 +2912,11 @@
         <f t="shared" si="0"/>
         <v>0.2540772568013866</v>
       </c>
-      <c r="V40" s="1"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V40" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2.0659976477696101E-2</v>
       </c>
@@ -2888,9 +2975,11 @@
         <f t="shared" si="0"/>
         <v>0.27122464040368799</v>
       </c>
-      <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V41" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2.025226724750458E-2</v>
       </c>
@@ -2949,9 +3038,11 @@
         <f t="shared" si="0"/>
         <v>0.22436898229575752</v>
       </c>
-      <c r="V42" s="1"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V42" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2.0210621870617441E-2</v>
       </c>
@@ -3010,9 +3101,11 @@
         <f t="shared" si="0"/>
         <v>0.32862344696267143</v>
       </c>
-      <c r="V43" s="1"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V43" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2.0282629124957593E-2</v>
       </c>
@@ -3071,9 +3164,11 @@
         <f t="shared" si="0"/>
         <v>0.32714440242476356</v>
       </c>
-      <c r="V44" s="1"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V44" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1.9927333795499737E-2</v>
       </c>
@@ -3132,9 +3227,11 @@
         <f t="shared" si="0"/>
         <v>0.27642375858345491</v>
       </c>
-      <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V45" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2.0005202338259871E-2</v>
       </c>
@@ -3193,9 +3290,11 @@
         <f t="shared" si="0"/>
         <v>0.28059455874117212</v>
       </c>
-      <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V46" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1.9992070448024042E-2</v>
       </c>
@@ -3254,9 +3353,11 @@
         <f t="shared" si="0"/>
         <v>0.28380923161772231</v>
       </c>
-      <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V47" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -3315,9 +3416,11 @@
         <f t="shared" si="0"/>
         <v>1.2876917532405798</v>
       </c>
-      <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V48" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1.9607843137278275E-2</v>
       </c>
@@ -3376,9 +3479,11 @@
         <f t="shared" si="0"/>
         <v>1.2971068485754387</v>
       </c>
-      <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V49" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1.9645457395348342E-2</v>
       </c>
@@ -3437,9 +3542,11 @@
         <f t="shared" si="0"/>
         <v>0.26932818503901662</v>
       </c>
-      <c r="V50" s="1"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V50" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1.9951738452798354E-2</v>
       </c>
@@ -3498,9 +3605,11 @@
         <f t="shared" si="0"/>
         <v>0.27145303336434567</v>
       </c>
-      <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V51" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1.9998843607435941E-2</v>
       </c>
@@ -3559,9 +3668,11 @@
         <f t="shared" si="0"/>
         <v>0.28654524646595997</v>
       </c>
-      <c r="V52" s="1"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V52" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2.0026451592428662E-2</v>
       </c>
@@ -3620,9 +3731,11 @@
         <f t="shared" si="0"/>
         <v>0.31884758180344047</v>
       </c>
-      <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V53" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -3681,9 +3794,11 @@
         <f t="shared" si="0"/>
         <v>1.589317295425493</v>
       </c>
-      <c r="V54" s="1"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V54" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1.9607843137277106E-2</v>
       </c>
@@ -3742,9 +3857,11 @@
         <f t="shared" si="0"/>
         <v>1.6462499301317335</v>
       </c>
-      <c r="V55" s="1"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V55" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2.0366570167200934E-2</v>
       </c>
@@ -3803,9 +3920,11 @@
         <f t="shared" si="0"/>
         <v>0.35377886976758738</v>
       </c>
-      <c r="V56" s="1"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V56" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2.0129219557690085E-2</v>
       </c>
@@ -3864,9 +3983,11 @@
         <f t="shared" si="0"/>
         <v>0.34584049212173767</v>
       </c>
-      <c r="V57" s="1"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V57" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2.0054592919120613E-2</v>
       </c>
@@ -3925,9 +4046,11 @@
         <f t="shared" si="0"/>
         <v>0.34198793700745322</v>
       </c>
-      <c r="V58" s="1"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V58" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2.0104950713402122E-2</v>
       </c>
@@ -3986,9 +4109,11 @@
         <f t="shared" si="0"/>
         <v>0.33537946719301537</v>
       </c>
-      <c r="V59" s="1"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V59" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2.0012780867335468E-2</v>
       </c>
@@ -4047,9 +4172,11 @@
         <f t="shared" si="0"/>
         <v>0.32884882038436647</v>
       </c>
-      <c r="V60" s="1"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V60" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1.9998083024111244E-2</v>
       </c>
@@ -4108,9 +4235,11 @@
         <f t="shared" si="0"/>
         <v>0.31613592387401462</v>
       </c>
-      <c r="V61" s="1"/>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V61" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1.9692249061837561E-2</v>
       </c>
@@ -4169,9 +4298,11 @@
         <f t="shared" si="0"/>
         <v>0.34286782715600805</v>
       </c>
-      <c r="V62" s="1"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V62" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1.9697513638395572E-2</v>
       </c>
@@ -4230,9 +4361,11 @@
         <f t="shared" si="0"/>
         <v>0.42696708328645028</v>
       </c>
-      <c r="V63" s="1"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V63" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1.9965157519024546E-2</v>
       </c>
@@ -4291,9 +4424,11 @@
         <f t="shared" si="0"/>
         <v>0.54411188581534764</v>
       </c>
-      <c r="V64" s="1"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V64" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1.9773462759084589E-2</v>
       </c>
@@ -4352,9 +4487,11 @@
         <f t="shared" si="0"/>
         <v>0.67551275472943106</v>
       </c>
-      <c r="V65" s="1"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V65" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2.0162262931169513E-2</v>
       </c>
@@ -4413,9 +4550,11 @@
         <f t="shared" ref="T66" si="1">SQRT(P66^2+Q66^2+R66^2)</f>
         <v>0.81052621562141847</v>
       </c>
-      <c r="V66" s="1"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V66" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0</v>
       </c>
@@ -4471,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
@@ -4527,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0</v>
       </c>
@@ -4583,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0</v>
       </c>
@@ -4639,7 +4778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0</v>
       </c>
@@ -4695,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0</v>
       </c>
@@ -4751,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0</v>
       </c>
@@ -4807,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0</v>
       </c>
@@ -4863,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0</v>
       </c>
@@ -4919,7 +5058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0</v>
       </c>
@@ -4975,7 +5114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0</v>
       </c>
@@ -5031,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0</v>
       </c>
@@ -5087,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0</v>
       </c>
@@ -5143,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0</v>
       </c>
@@ -5199,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0</v>
       </c>
@@ -5255,7 +5394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0</v>
       </c>
@@ -5311,7 +5450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0</v>
       </c>
@@ -5367,7 +5506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0</v>
       </c>
@@ -5423,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0</v>
       </c>
@@ -5479,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0</v>
       </c>
@@ -5535,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0</v>
       </c>
@@ -5591,7 +5730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0</v>
       </c>
@@ -5647,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0</v>
       </c>
@@ -5703,7 +5842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0</v>
       </c>
@@ -5759,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0</v>
       </c>
@@ -5815,7 +5954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0</v>
       </c>
@@ -5871,7 +6010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0</v>
       </c>
@@ -5927,7 +6066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0</v>
       </c>
@@ -5983,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0</v>
       </c>
@@ -6039,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -6095,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0</v>
       </c>
@@ -6151,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0</v>
       </c>
@@ -6207,7 +6346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0</v>
       </c>
@@ -6263,7 +6402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0</v>
       </c>
@@ -6319,7 +6458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0</v>
       </c>
@@ -6375,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
@@ -6431,7 +6570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0</v>
       </c>
@@ -6487,7 +6626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -6543,7 +6682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -6599,7 +6738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -6655,7 +6794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -6711,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0</v>
       </c>
@@ -6767,7 +6906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -6823,7 +6962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -6879,7 +7018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -6935,7 +7074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -6991,7 +7130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -7047,7 +7186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -7103,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0</v>
       </c>
@@ -7159,7 +7298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -7215,7 +7354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0</v>
       </c>
@@ -7271,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0</v>
       </c>
@@ -7327,7 +7466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -7383,7 +7522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -7439,7 +7578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0</v>
       </c>
@@ -7495,7 +7634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0</v>
       </c>
@@ -7551,7 +7690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0</v>
       </c>
@@ -7607,7 +7746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0</v>
       </c>
@@ -7663,7 +7802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0</v>
       </c>
@@ -7719,7 +7858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0</v>
       </c>
@@ -7775,7 +7914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0</v>
       </c>
@@ -7831,7 +7970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0</v>
       </c>
@@ -7887,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0</v>
       </c>
@@ -7943,7 +8082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0</v>
       </c>
@@ -7999,7 +8138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0</v>
       </c>
@@ -8055,7 +8194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0</v>
       </c>

</xml_diff>